<commit_message>
Alterações na página de captura do Selenium
</commit_message>
<xml_diff>
--- a/excel/Arquivo - Copia - Copia - Copia.xlsx
+++ b/excel/Arquivo - Copia - Copia - Copia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>Torneio</t>
   </si>
@@ -26,11 +26,18 @@
   <si>
     <t>pokerstars</t>
   </si>
+  <si>
+    <t>35835,31</t>
+  </si>
+  <si>
+    <t>17919,61</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,8 +396,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -402,60 +409,72 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>2</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401">
+      <c r="A401" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B401" t="s">
+      <c r="B401" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C401">
+      <c r="C401" s="0">
         <v>8358</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402">
+      <c r="A402" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B402" t="s">
+      <c r="B402" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C402">
+      <c r="C402" s="0">
         <v>16712</v>
       </c>
-      <c r="D402">
+      <c r="D402" s="0">
         <v>8354</v>
       </c>
-      <c r="E402">
+      <c r="E402" s="0">
         <v>8358</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A801">
+      <c r="A801" s="0">
         <v>3540607900</v>
       </c>
-      <c r="B801" t="s">
+      <c r="B801" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C801">
+      <c r="C801" s="0">
         <v>8358</v>
       </c>
     </row>

</xml_diff>